<commit_message>
Versión inicial de actualización de datos de trabajadores por lote
</commit_message>
<xml_diff>
--- a/src/app/00078-GestionPlanillas/WebApp/Assets/application/formatos/Catalogo del formato de carga de trabajadores.xlsx
+++ b/src/app/00078-GestionPlanillas/WebApp/Assets/application/formatos/Catalogo del formato de carga de trabajadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\repos\00078-DWeb_GestionPlanillas\src\app\00078-GestionPlanillas\WebApp\Assets\application\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10311098-05B5-4165-9E74-5DD9EF4B3F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E345ACFD-83BB-4548-A95A-D1B38489111B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A22229E-7FFA-4F20-BBFA-6FC8C3493951}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="606">
   <si>
     <t>Tipo de Documento</t>
   </si>
@@ -1847,6 +1847,15 @@
   </si>
   <si>
     <t>Profuturo AFP</t>
+  </si>
+  <si>
+    <t>Acción</t>
+  </si>
+  <si>
+    <t>registrar</t>
+  </si>
+  <si>
+    <t>actualizar</t>
   </si>
 </sst>
 </file>
@@ -1911,7 +1920,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1943,6 +1952,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2257,7 +2268,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{812619F6-F5F8-4389-8046-263F945FDC1D}">
-  <dimension ref="A1:B106"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2267,664 +2278,681 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="18" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>1</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
         <v>2</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>35</v>
+      <c r="A24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
         <v>1</v>
       </c>
-      <c r="B31" s="8"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
+      <c r="B35" s="8"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
         <v>2</v>
       </c>
-      <c r="B32" s="8"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
+      <c r="B36" s="8"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
         <v>3</v>
       </c>
-      <c r="B33" s="8"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
         <v>4</v>
-      </c>
-      <c r="B34" s="8"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="8"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="8"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="8"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="B38" s="8"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="8"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="8"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="8"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="8"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="8"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+      <c r="B43" s="8"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B54" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B55" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B56" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="6">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
         <v>1</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B57" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="6">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
         <v>2</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B58" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="6">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
         <v>3</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B59" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
-        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="6">
-        <v>0</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="6">
-        <v>1</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="6">
-        <v>2</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="6">
-        <v>3</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
+        <v>3</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="6">
+        <v>5</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="6">
+        <v>6</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="6">
+        <v>7</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="6">
         <v>8</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B86" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="14" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="14" t="s">
         <v>585</v>
       </c>
-      <c r="B87" s="15" t="s">
+      <c r="B91" s="15" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
         <v>597</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="6">
-        <v>1</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="6">
-        <v>2</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="6">
-        <v>3</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="6">
-        <v>4</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="6">
+        <v>2</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="6">
+        <v>3</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="6">
+        <v>4</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="6">
+        <v>6</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="6">
         <v>9</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>591</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="9" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="9" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="16">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="16">
         <v>1</v>
       </c>
-      <c r="B103" s="6" t="s">
+      <c r="B107" s="6" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="16">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="16">
         <v>2</v>
       </c>
-      <c r="B104" s="6" t="s">
+      <c r="B108" s="6" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="16">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="16">
         <v>3</v>
       </c>
-      <c r="B105" s="6" t="s">
+      <c r="B109" s="6" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="16">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="16">
         <v>4</v>
       </c>
-      <c r="B106" s="6" t="s">
+      <c r="B110" s="6" t="s">
         <v>602</v>
       </c>
     </row>

</xml_diff>

<commit_message>
actualización manual y formatos
</commit_message>
<xml_diff>
--- a/src/app/00078-GestionPlanillas/WebApp/Assets/application/formatos/Catalogo del formato de carga de trabajadores.xlsx
+++ b/src/app/00078-GestionPlanillas/WebApp/Assets/application/formatos/Catalogo del formato de carga de trabajadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\repos\00078-DWeb_GestionPlanillas\src\app\00078-GestionPlanillas\WebApp\Assets\application\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E345ACFD-83BB-4548-A95A-D1B38489111B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9163D8-ECAF-43E5-803B-A2EFC747CFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A22229E-7FFA-4F20-BBFA-6FC8C3493951}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="608">
   <si>
     <t>Tipo de Documento</t>
   </si>
@@ -1852,10 +1852,16 @@
     <t>Acción</t>
   </si>
   <si>
-    <t>registrar</t>
-  </si>
-  <si>
-    <t>actualizar</t>
+    <t>Registrar</t>
+  </si>
+  <si>
+    <t>Actualizar</t>
+  </si>
+  <si>
+    <t>registrar nuevo trabajador</t>
+  </si>
+  <si>
+    <t>actualizar información de un trabajador</t>
   </si>
 </sst>
 </file>
@@ -1920,7 +1926,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1952,8 +1958,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2278,7 +2282,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="7" t="s">
         <v>603</v>
       </c>
     </row>
@@ -2286,16 +2290,20 @@
       <c r="A2" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>607</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1"/>

</xml_diff>